<commit_message>
Se agrego campo 'Fue grabada' en Clases, actualizamos todo el programa + modelos
</commit_message>
<xml_diff>
--- a/PuntajeClases/BackUps/Back up 24_03_2021__05hs_22mins.xlsx
+++ b/PuntajeClases/BackUps/Back up 24_03_2021__05hs_22mins.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matia\source\repos\Sol_Puntaje\PuntajeClases\BackUps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{46DA5570-46BD-4D1D-AF53-B3B9B8ED924C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F05346B6-8471-4489-8A82-91A8AD0FBABA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="8964" xr2:uid="{9C3A99DA-294E-4B34-B40E-513E42A15CF2}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{9C3A99DA-294E-4B34-B40E-513E42A15CF2}"/>
   </bookViews>
   <sheets>
     <sheet name="Materias" sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="113">
   <si>
     <t>Dia Clase</t>
   </si>
@@ -368,16 +368,28 @@
   </si>
   <si>
     <t>Hinojosa Pablo</t>
+  </si>
+  <si>
+    <t>Año</t>
+  </si>
+  <si>
+    <t>Periodo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -722,7 +734,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AF1582F-E685-4CB2-866E-1C31A79AED7C}">
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -738,6 +752,12 @@
       </c>
       <c r="D1" t="s">
         <v>86</v>
+      </c>
+      <c r="E1" t="s">
+        <v>111</v>
+      </c>
+      <c r="F1" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -942,7 +962,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C48A311-A8D2-46B4-ACC5-F377D6835FED}">
   <dimension ref="A1:D47"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection sqref="A1:D47"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -1605,6 +1627,8 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>